<commit_message>
Added tasks 33 and 34
</commit_message>
<xml_diff>
--- a/решение С#.xlsx
+++ b/решение С#.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1035442\OneDrive - Syngenta\Рабочий стол\Geek Brains\C# Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3EE5A4-3004-465F-997C-CDECB66295E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F2DAA0-2446-4037-9798-8013DB9BBB33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C4871C03-24D8-4764-B569-A8F27D0CFEA3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
   <si>
     <t>02 Написать программу которая на вход принимает два числа и выводит, какое число большее, а какое меньшее.</t>
   </si>
@@ -1288,8 +1288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98C62B4D-52C8-429E-A392-6844393624AA}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1855,13 +1855,16 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B36" s="6">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>56</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="150" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Solved a lot of tasks
</commit_message>
<xml_diff>
--- a/решение С#.xlsx
+++ b/решение С#.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1035442\OneDrive - Syngenta\Рабочий стол\Geek Brains\C# Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F2DAA0-2446-4037-9798-8013DB9BBB33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{98C9A430-18C3-49B9-A1E9-E5519D2A5E75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C4871C03-24D8-4764-B569-A8F27D0CFEA3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{C4871C03-24D8-4764-B569-A8F27D0CFEA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="85">
   <si>
     <t>02 Написать программу которая на вход принимает два числа и выводит, какое число большее, а какое меньшее.</t>
   </si>
@@ -889,6 +890,321 @@
 PrintArray(userArray);
 System.Console.WriteLine($"Is searching number {userSearchNumber} available in random array: {CheckNumberInArray(userArray, userSearchNumber)}");
 </t>
+  </si>
+  <si>
+    <t>using System;
+public class Answer
+{
+    public static int SumOddElements(int[] array)
+    {
+        // Введите свое решение ниже
+        int result = 0;
+        for (int i = 1; i &lt; array.Length; i ++)
+        {
+            if(i%2 !=0) result = result + array[i];
+        }
+        return result;
+    }
+    public static void PrintArray(int[] array)
+    {
+        // Введите свое решение ниже
+    for (int i = 0; i &lt; array.Length; i++)
+    {
+        Console.Write(array[i]);
+        if(i&lt; array.Length - 1) Console.Write("\t");
+    }
+    System.Console.WriteLine("");
+    }
+    // Не удаляйте и не меняйте метод Main! 
+    public static void Main(string[] args)
+    {
+        int[] array;
+        if (args.Length == 0)
+        {
+            // Здесь вы можете поменять значения для отправки кода на Выполнение
+            array = new int[] { 18, 76, 11 };
+        }
+        else
+        {
+            string[] argStrings = args[0].Split(", ");
+            array = new int[argStrings.Length];
+            for (int i = 0; i &lt; argStrings.Length; i++)
+            {
+                if (int.TryParse(argStrings[i], out int number))
+                {
+                    array[i] = number;
+                }
+                else
+                {
+                    Console.WriteLine($"Ошибка при парсинге аргумента {argStrings[i]}.");
+                    return;
+                }
+            }
+        }
+        // Не удаляйте строки ниже
+        PrintArray(array);
+        int sumOdd = SumOddElements(array);
+        Console.WriteLine($"Сумма нечетных элементов: {sumOdd}");
+    }
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/*
+35. Задайте одномерный массив из 123 случайных чисел. Найдите количество элементов массива, 
+значения которых лежат в отрезке [10,99]. 
+Пример для массива из 5, а не 123 элементов. В своем решении 
+сделайте для 123
+[5, 18, 123, 6, 2] -&gt; 1
+[1, 2, 3, 6, 2] -&gt; 0
+[10, 11, 12, 13, 14] -&gt; 5
+*/
+using System;
+Console.Clear();
+int[] GetRandomArray(int start, int end, int lenght)
+{
+    int[] array = new int[lenght];
+    for (int i = 0; i &lt; lenght; i++)
+    {
+        array[i] = new Random().Next(start, end+1);
+    }
+    return array;
+}
+void PrintArray(int[] array)
+{
+    System.Console.Write("[");
+    for (int i = 0; i &lt; array.Length; i++)
+    {
+        System.Console.Write(array[i]);
+        if (i &lt; array.Length - 1)
+            System.Console.Write(", ");
+    }
+    System.Console.WriteLine("]");
+}
+int TakeEntNum(string message)
+{
+    System.Console.WriteLine(message);
+    int result = Convert.ToInt32(Console.ReadLine());
+    return result;
+}
+int SumPositiveNum (int[] array)
+{
+ int result = 0;
+ for (int i = 0; i &lt; array.Length; i++)
+ {
+    if (array[i] &gt; 0) result +=array[i];
+ }
+ return result;
+}
+int SumNegativeNum (int[] array)
+{
+ int result = 0;
+ for (int i = 0; i &lt; array.Length; i++)
+ {
+    if (array[i] &lt; 0) result +=array[i];
+ }
+ return result;
+}
+int FindNumbersInRange (int[] array, int start, int end)
+{
+    int count = 0;    
+    for (int i = 0; i &lt; array.Length; i++)
+    {
+        if(array[i] &gt; start &amp;&amp; array[i] &lt; end + 1  ) count++;
+    }
+    return count;
+}
+int userArraySize = TakeEntNum ("Please, enter array size:");
+int userArrayStart = TakeEntNum ("Please, enter array start number range:");
+int userArrayEnd =  TakeEntNum ("Please, enter array end number range:");
+int[] userArray = GetRandomArray (userArrayStart, userArrayEnd, userArraySize);
+PrintArray (userArray);
+int userRangeStartFind = TakeEntNum("Enter the start of range to find numbers in given Array: ");
+int userRangeEndFind = TakeEntNum ("Enter the start of range to find numbers in given Array: ");
+int  userRangeCountInArray = FindNumbersInRange(userArray, userRangeStartFind, userRangeEndFind);
+System.Console.WriteLine($"Counted numbers in given range in curent array: {FindNumbersInRange(userArray, userRangeStartFind, userRangeEndFind)}. ");
+ </t>
+  </si>
+  <si>
+    <t>/*
+38. Напишите программу для работы с массивом вещественных чисел.
+Аргументы, передаваемые в метод/функцию:
+'3.17, 8.94, 2.36, 5.72, 0.85'
+На выходе:
+Массив:
+3.17    8.94    2.36    5.72    0.85    
+Разность между максимальным и минимальным элементом = 8.09
+*/
+using System;
+public class Answer
+{
+    public static double FindMax(double[] array)
+    {     // Введите свое решение ниже
+        double max = array[0];
+        for (int i = 0; i &lt; array.Length; i++)
+        {
+            if (array[i] &gt; max) max = array[i];
+        }
+        return max;
+    }
+    public static double FindMin(double[] array)
+    {     // Введите свое решение ниже
+        double min = array[0];
+        for (int i = 0; i &lt; array.Length; i++)
+        {
+            if (array[i] &lt; min) min = array[i];
+        }
+        return min;
+    }
+    public static double CalcDifferenceBetweenMaxMin(double[] array)
+    {// Введите свое решение ниже
+        double max = FindMax(array);
+        double min = FindMin(array);
+        double diff = max - min;
+        return diff;
+    }
+    public static void PrintArray(double[] array)
+    {
+        for (int i = 0; i &lt; array.Length; i++)
+        {
+            Console.Write(array[i]);
+            if(i &lt; array.Length - 1) Console.Write ("\t");
+        }
+        System.Console.WriteLine("");
+    }
+    // Не удаляйте и не меняйте метод Main! 
+    public static void Main(string[] args)
+    {
+        double[] array;
+        if (args.Length == 0)
+        {
+            array = new double[] { 3, 7.4, 22.3, 2, 78 };
+        }
+        else
+        {
+            // Иначе, парсим аргументы в массив чисел
+            string[] argStrings = args[0].Split(", ");
+            array = new double[argStrings.Length];
+            for (int i = 0; i &lt; argStrings.Length; i++)
+            {
+                if (double.TryParse(argStrings[i], out double number))
+                {
+                    array[i] = number;
+                }
+                else
+                {
+                    Console.WriteLine($"Ошибка при парсинге аргумента {argStrings[i]}.");
+                    return;
+                }
+            }
+        }
+        Console.WriteLine("Массив:");
+        PrintArray(array);
+        double diff = CalcDifferenceBetweenMaxMin(array);
+        Console.WriteLine($"Разность между максимальным и минимальным элементом = {diff:f2}");
+    }
+}</t>
+  </si>
+  <si>
+    <t>/*
+21 Напишите программу, которая принимает на вход координаты двух точек и находит расстояние между ними в 3D пространстве.
+*/
+using System;
+Console.Clear();
+string TakeEntCoordinate(string message)
+{
+    System.Console.WriteLine(message);
+    string result = Convert.ToString(Console.ReadLine());
+    return result;
+}
+double DistanceBetweenPointsIn2D(int[] a, int[] b)
+{
+    double result = 0;
+    for (int i = 0; i &lt; a.Length; i++)
+    {
+        result = result + Math.Pow((a[i] - b[i]), 2);
+    }
+    return result = Math.Sqrt(result);
+}
+string inputA = TakeEntCoordinate("Enter Coordinate of first point splited by space button (x y):");
+var strings1 = inputA.Split(' ');
+int[] pointA = Array.ConvertAll(strings1, s =&gt; int.Parse(s));
+string inputB = TakeEntCoordinate("Enter Coordinate of first point splited by space button (x y):");
+var strings2 = inputB.Split(' ');
+int[] pointB = Array.ConvertAll(strings2, s =&gt; int.Parse(s));
+System.Console.WriteLine($"Distance beetween of two entered point is: {DistanceBetweenPointsIn2D(pointA, pointB)}");</t>
+  </si>
+  <si>
+    <t>/*
+21 Напишите программу, которая принимает на вход координаты двух точек и находит расстояние между ними в 3D пространстве.
+*/
+using System;
+Console.Clear();
+string TakeEntCoordinate(string message)
+{
+    System.Console.WriteLine(message);
+    string result = Convert.ToString(Console.ReadLine());
+    return result;
+}
+double DistanceBetweenPointsIn3D(int[] a, int[] b)
+{
+    double result = 0;
+    for (int i = 0; i &lt; 3; i++)
+    {
+        result = result + Math.Pow((a[i] - b[i]), 2);
+    }
+    return result = Math.Sqrt(result);
+}
+string inputA = TakeEntCoordinate("Enter Coordinate of first point splited by space button (x y z):");
+var strings1 = inputA.Split(' ');
+int[] pointA = Array.ConvertAll(strings1, s =&gt; int.Parse(s));
+string inputB = TakeEntCoordinate("Enter Coordinate of first point splited by space button (x y z):");
+var strings2 = inputB.Split(' ');
+int[] pointB = Array.ConvertAll(strings2, s =&gt; int.Parse(s));
+System.Console.WriteLine($"Distance beetween of two entered point is: {DistanceBetweenPointsIn3D(pointA, pointB)}");</t>
+  </si>
+  <si>
+    <t>/*
+22 Напишите программу, которая принимает на вход число(N) и выдаёт таблицу квадратов чисел от 1 до N.
+*/
+using System;
+Console.Clear();
+void PrintSquareNumber(int a)
+{
+    for (int i = 1; i &lt;= a; i++)
+    {
+        System.Console.WriteLine($"{i} * {i} = {Math.Pow(i,2)}");
+    }
+    }
+int TakeEntNum(string message)
+{
+    System.Console.WriteLine(message);
+    int result = Convert.ToInt32(Console.ReadLine());
+    return result;
+}
+int userNumber1 = TakeEntNum("Enter number for calculation: ");
+PrintSquareNumber(userNumber1);</t>
+  </si>
+  <si>
+    <t>/*
+23 Напишите программу, которая принимает на вход число (N) и выдаёт таблицу кубов чисел от 1 до N.
+*/
+using System;
+Console.Clear();
+void PrintSquareNumber(int a)
+{
+    for (int i = 1; i &lt;= a; i++)
+    {
+        System.Console.WriteLine($"{i} * {i} * {i}= {Math.Pow(i,3)}");
+    }
+    }
+int TakeEntNum(string message)
+{
+    System.Console.WriteLine(message);
+    int result = Convert.ToInt32(Console.ReadLine());
+    return result;
+}
+int userNumber1 = TakeEntNum("Enter number for calculation: ");
+PrintSquareNumber(userNumber1);</t>
   </si>
 </sst>
 </file>
@@ -939,7 +1255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -962,9 +1278,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1288,8 +1601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98C62B4D-52C8-429E-A392-6844393624AA}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,7 +1610,7 @@
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
     <col min="3" max="3" width="44.5703125" customWidth="1"/>
-    <col min="4" max="4" width="188.42578125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="188.42578125" style="9" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1323,12 +1636,12 @@
       <c r="C2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="8" t="s">
         <v>25</v>
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="345" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <f t="shared" ref="A3:B25" si="0">A2+1</f>
         <v>1</v>
@@ -1340,7 +1653,7 @@
       <c r="C3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
       <c r="E3" s="2"/>
@@ -1583,7 +1896,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="390" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1595,12 +1908,12 @@
       <c r="C18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="8" t="s">
         <v>67</v>
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1612,12 +1925,12 @@
       <c r="C19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="285" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1629,12 +1942,12 @@
       <c r="C20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="8" t="s">
         <v>69</v>
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1646,12 +1959,12 @@
       <c r="C21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="8" t="s">
         <v>51</v>
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1663,10 +1976,12 @@
       <c r="C22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="8"/>
+      <c r="D22" s="5" t="s">
+        <v>81</v>
+      </c>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1678,10 +1993,12 @@
       <c r="C23" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="8"/>
+      <c r="D23" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="360" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1693,10 +2010,12 @@
       <c r="C24" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="8"/>
+      <c r="D24" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="360" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1708,10 +2027,12 @@
       <c r="C25" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="8"/>
+      <c r="D25" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" ht="255" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -1722,11 +2043,11 @@
       <c r="C26" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>24</v>
       </c>
@@ -1737,11 +2058,11 @@
       <c r="C27" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="390" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>25</v>
       </c>
@@ -1752,11 +2073,11 @@
       <c r="C28" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>26</v>
       </c>
@@ -1767,11 +2088,11 @@
       <c r="C29" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="9" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="345" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>27</v>
       </c>
@@ -1782,11 +2103,11 @@
       <c r="C30" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D30" s="9" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>28</v>
       </c>
@@ -1797,11 +2118,11 @@
       <c r="C31" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>29</v>
       </c>
@@ -1812,11 +2133,11 @@
       <c r="C32" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="9" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>30</v>
       </c>
@@ -1827,11 +2148,11 @@
       <c r="C33" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D33" s="9" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="B34" s="6">
         <f t="shared" si="1"/>
         <v>32</v>
@@ -1839,11 +2160,11 @@
       <c r="C34" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="11" t="s">
+      <c r="D34" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B35" s="6">
         <f t="shared" si="1"/>
         <v>33</v>
@@ -1851,11 +2172,11 @@
       <c r="C35" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="B36" s="6">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -1863,11 +2184,11 @@
       <c r="C36" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="D36" s="9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B37" s="6">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -1875,8 +2196,11 @@
       <c r="C37" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="D37" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B38" s="6">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -1884,6 +2208,9 @@
       <c r="C38" s="3" t="s">
         <v>54</v>
       </c>
+      <c r="D38" s="10" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="39" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="B39" s="6">
@@ -1894,13 +2221,16 @@
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B40" s="6">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>52</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="105" x14ac:dyDescent="0.25">
@@ -2059,5 +2389,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
</xml_diff>